<commit_message>
cleaning up crab correlation matrix
</commit_message>
<xml_diff>
--- a/data/jho_temporal_data_summarized.xlsx
+++ b/data/jho_temporal_data_summarized.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="raw data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="35">
   <si>
     <t>year</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t>water_temperature</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>cogg</t>
+  </si>
+  <si>
+    <t>nag</t>
   </si>
 </sst>
 </file>
@@ -442,39 +451,39 @@
   <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:T12"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="1"/>
     <col min="5" max="5" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
     <col min="8" max="9" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" style="1"/>
     <col min="16" max="16" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.88671875" style="1"/>
+    <col min="18" max="18" width="8.85546875" style="1"/>
     <col min="19" max="19" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.88671875" style="1"/>
+    <col min="21" max="21" width="8.85546875" style="1"/>
     <col min="22" max="22" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.88671875" style="1"/>
+    <col min="26" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +542,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2010</v>
       </c>
@@ -592,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2011</v>
       </c>
@@ -645,7 +654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2012</v>
       </c>
@@ -704,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2013</v>
       </c>
@@ -763,7 +772,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2014</v>
       </c>
@@ -816,7 +825,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2015</v>
       </c>
@@ -875,7 +884,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E8" s="1">
         <v>2010</v>
       </c>
@@ -925,7 +934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E9" s="1">
         <v>2011</v>
       </c>
@@ -975,7 +984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E10" s="1">
         <v>2012</v>
       </c>
@@ -1025,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E11" s="1">
         <v>2013</v>
       </c>
@@ -1075,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E12" s="1">
         <v>2014</v>
       </c>
@@ -1125,7 +1134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F13" s="2"/>
       <c r="I13" s="1">
         <v>2009</v>
@@ -1161,7 +1170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F14" s="2"/>
       <c r="I14" s="1">
         <v>2010</v>
@@ -1197,7 +1206,7 @@
         <v>10.666700000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F15" s="2"/>
       <c r="I15" s="1">
         <v>2011</v>
@@ -1233,7 +1242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F16" s="2"/>
       <c r="I16" s="1">
         <v>2012</v>
@@ -1269,7 +1278,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:25" x14ac:dyDescent="0.25">
       <c r="F17" s="2"/>
       <c r="I17" s="1">
         <v>2013</v>
@@ -1305,7 +1314,7 @@
         <v>26.666699999999999</v>
       </c>
     </row>
-    <row r="18" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:25" x14ac:dyDescent="0.25">
       <c r="F18" s="2"/>
       <c r="I18" s="1">
         <v>2014</v>
@@ -1335,7 +1344,7 @@
         <v>13.333299999999999</v>
       </c>
     </row>
-    <row r="19" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:25" x14ac:dyDescent="0.25">
       <c r="I19" s="1">
         <v>2015</v>
       </c>
@@ -1358,7 +1367,7 @@
         <v>13.333299999999999</v>
       </c>
     </row>
-    <row r="20" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:25" x14ac:dyDescent="0.25">
       <c r="V20" s="1" t="s">
         <v>11</v>
       </c>
@@ -1372,7 +1381,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:25" x14ac:dyDescent="0.25">
       <c r="V21" s="1" t="s">
         <v>11</v>
       </c>
@@ -1386,7 +1395,7 @@
         <v>37.333300000000001</v>
       </c>
     </row>
-    <row r="22" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:25" x14ac:dyDescent="0.25">
       <c r="V22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1400,7 +1409,7 @@
         <v>73.333299999999994</v>
       </c>
     </row>
-    <row r="23" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:25" x14ac:dyDescent="0.25">
       <c r="V23" s="1" t="s">
         <v>11</v>
       </c>
@@ -1414,7 +1423,7 @@
         <v>2.6667000000000001</v>
       </c>
     </row>
-    <row r="24" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:25" x14ac:dyDescent="0.25">
       <c r="V24" s="1" t="s">
         <v>11</v>
       </c>
@@ -1428,7 +1437,7 @@
         <v>1.3332999999999999</v>
       </c>
     </row>
-    <row r="25" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:25" x14ac:dyDescent="0.25">
       <c r="V25" s="1" t="s">
         <v>11</v>
       </c>
@@ -1442,7 +1451,7 @@
         <v>105.33329999999999</v>
       </c>
     </row>
-    <row r="26" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="6:25" x14ac:dyDescent="0.25">
       <c r="V26" s="1" t="s">
         <v>11</v>
       </c>
@@ -1456,7 +1465,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="6:25" x14ac:dyDescent="0.25">
       <c r="V27" s="1" t="s">
         <v>11</v>
       </c>
@@ -1470,7 +1479,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="6:25" x14ac:dyDescent="0.25">
       <c r="V28" s="1" t="s">
         <v>11</v>
       </c>
@@ -1484,7 +1493,7 @@
         <v>21.333300000000001</v>
       </c>
     </row>
-    <row r="29" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="6:25" x14ac:dyDescent="0.25">
       <c r="V29" s="1" t="s">
         <v>14</v>
       </c>
@@ -1498,7 +1507,7 @@
         <v>1.3332999999999999</v>
       </c>
     </row>
-    <row r="30" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="6:25" x14ac:dyDescent="0.25">
       <c r="V30" s="1" t="s">
         <v>14</v>
       </c>
@@ -1512,7 +1521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="6:25" x14ac:dyDescent="0.25">
       <c r="V31" s="1" t="s">
         <v>14</v>
       </c>
@@ -1526,7 +1535,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="6:25" x14ac:dyDescent="0.25">
       <c r="V32" s="1" t="s">
         <v>14</v>
       </c>
@@ -1540,7 +1549,7 @@
         <v>173.33330000000001</v>
       </c>
     </row>
-    <row r="33" spans="22:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="22:25" x14ac:dyDescent="0.25">
       <c r="V33" s="1" t="s">
         <v>14</v>
       </c>
@@ -1554,7 +1563,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="22:25" x14ac:dyDescent="0.3">
+    <row r="34" spans="22:25" x14ac:dyDescent="0.25">
       <c r="V34" s="1" t="s">
         <v>14</v>
       </c>
@@ -1568,7 +1577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="22:25" x14ac:dyDescent="0.3">
+    <row r="35" spans="22:25" x14ac:dyDescent="0.25">
       <c r="V35" s="1" t="s">
         <v>14</v>
       </c>
@@ -1582,7 +1591,7 @@
         <v>6.6666999999999996</v>
       </c>
     </row>
-    <row r="36" spans="22:25" x14ac:dyDescent="0.3">
+    <row r="36" spans="22:25" x14ac:dyDescent="0.25">
       <c r="V36" s="1" t="s">
         <v>14</v>
       </c>
@@ -1596,7 +1605,7 @@
         <v>6.6666999999999996</v>
       </c>
     </row>
-    <row r="37" spans="22:25" x14ac:dyDescent="0.3">
+    <row r="37" spans="22:25" x14ac:dyDescent="0.25">
       <c r="V37" s="1" t="s">
         <v>14</v>
       </c>
@@ -1610,7 +1619,7 @@
         <v>37.333300000000001</v>
       </c>
     </row>
-    <row r="38" spans="22:25" x14ac:dyDescent="0.3">
+    <row r="38" spans="22:25" x14ac:dyDescent="0.25">
       <c r="V38" s="1" t="s">
         <v>14</v>
       </c>
@@ -1624,7 +1633,7 @@
         <v>33.333300000000001</v>
       </c>
     </row>
-    <row r="39" spans="22:25" x14ac:dyDescent="0.3">
+    <row r="39" spans="22:25" x14ac:dyDescent="0.25">
       <c r="V39" s="1" t="s">
         <v>14</v>
       </c>
@@ -1638,7 +1647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="22:25" x14ac:dyDescent="0.3">
+    <row r="40" spans="22:25" x14ac:dyDescent="0.25">
       <c r="V40" s="1" t="s">
         <v>14</v>
       </c>
@@ -1652,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="22:25" x14ac:dyDescent="0.3">
+    <row r="41" spans="22:25" x14ac:dyDescent="0.25">
       <c r="V41" s="1" t="s">
         <v>14</v>
       </c>
@@ -1666,7 +1675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="22:25" x14ac:dyDescent="0.3">
+    <row r="42" spans="22:25" x14ac:dyDescent="0.25">
       <c r="V42" s="1" t="s">
         <v>14</v>
       </c>
@@ -1680,7 +1689,7 @@
         <v>37.333300000000001</v>
       </c>
     </row>
-    <row r="43" spans="22:25" x14ac:dyDescent="0.3">
+    <row r="43" spans="22:25" x14ac:dyDescent="0.25">
       <c r="V43" s="1" t="s">
         <v>14</v>
       </c>
@@ -1701,26 +1710,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H111"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="1"/>
-    <col min="6" max="6" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="11" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1731,19 +1741,13 @@
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1998</v>
       </c>
@@ -1753,20 +1757,14 @@
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="1">
-        <v>2010</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1998</v>
       </c>
@@ -1776,20 +1774,14 @@
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="1">
-        <v>2010</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1998</v>
       </c>
@@ -1799,20 +1791,14 @@
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="1">
-        <v>2012</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="1">
-        <v>2.88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1998</v>
       </c>
@@ -1822,20 +1808,14 @@
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1">
         <v>17</v>
       </c>
-      <c r="F5" s="1">
-        <v>2012</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1998</v>
       </c>
@@ -1845,20 +1825,14 @@
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1">
         <v>18</v>
       </c>
-      <c r="F6" s="1">
-        <v>2013</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="1">
-        <v>2.84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1998</v>
       </c>
@@ -1868,20 +1842,14 @@
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="1">
-        <v>2013</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1.83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E7" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1998</v>
       </c>
@@ -1891,20 +1859,14 @@
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1">
         <v>4</v>
       </c>
-      <c r="F8" s="1">
-        <v>2015</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="1">
-        <v>5.46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1998</v>
       </c>
@@ -1914,20 +1876,14 @@
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="1">
         <v>0</v>
       </c>
-      <c r="F9" s="1">
-        <v>2015</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="1">
-        <v>2.87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1998</v>
       </c>
@@ -1937,20 +1893,15 @@
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="1">
-        <v>2004</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="2">
-        <v>928879</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1998</v>
       </c>
@@ -1960,20 +1911,15 @@
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" s="1">
-        <v>2005</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="2">
-        <v>1024712</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1998</v>
       </c>
@@ -1983,20 +1929,15 @@
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="1">
-        <v>2006</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="2">
-        <v>930173</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1998</v>
       </c>
@@ -2006,20 +1947,15 @@
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="1">
         <v>0</v>
       </c>
-      <c r="F13" s="1">
-        <v>2007</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="2">
-        <v>876711</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2014</v>
       </c>
@@ -2029,20 +1965,15 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="1">
         <v>10.666700000000001</v>
       </c>
-      <c r="F14" s="1">
-        <v>2008</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="2">
-        <v>924396</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2014</v>
       </c>
@@ -2052,20 +1983,15 @@
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="1">
         <v>24</v>
       </c>
-      <c r="F15" s="1">
-        <v>2009</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="2">
-        <v>642860</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2014</v>
       </c>
@@ -2075,20 +2001,15 @@
       <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="1">
         <v>96</v>
       </c>
-      <c r="F16" s="1">
-        <v>2010</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="2">
-        <v>873044</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2014</v>
       </c>
@@ -2098,20 +2019,15 @@
       <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="1">
         <v>26.666699999999999</v>
       </c>
-      <c r="F17" s="1">
-        <v>2011</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="2">
-        <v>666209</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2014</v>
       </c>
@@ -2121,20 +2037,15 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="1">
         <v>13.333299999999999</v>
       </c>
-      <c r="F18" s="1">
-        <v>2012</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" s="2">
-        <v>693020</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2014</v>
       </c>
@@ -2144,20 +2055,15 @@
       <c r="C19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="1">
         <v>13.333299999999999</v>
       </c>
-      <c r="F19" s="1">
-        <v>2013</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="2">
-        <v>919883</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2014</v>
       </c>
@@ -2167,20 +2073,15 @@
       <c r="C20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="1">
         <v>36</v>
       </c>
-      <c r="F20" s="1">
-        <v>2014</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20" s="2">
-        <v>636412</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2014</v>
       </c>
@@ -2190,20 +2091,14 @@
       <c r="C21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="1">
         <v>37.333300000000001</v>
       </c>
-      <c r="F21" s="1">
-        <v>2004</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21" s="1">
-        <v>654970</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2014</v>
       </c>
@@ -2213,20 +2108,14 @@
       <c r="C22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="1">
         <v>73.333299999999994</v>
       </c>
-      <c r="F22" s="1">
-        <v>2005</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22" s="1">
-        <v>741061</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2014</v>
       </c>
@@ -2236,20 +2125,14 @@
       <c r="C23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="1">
         <v>2.6667000000000001</v>
       </c>
-      <c r="F23" s="1">
-        <v>2006</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H23" s="1">
-        <v>689075</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2014</v>
       </c>
@@ -2259,20 +2142,14 @@
       <c r="C24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="1">
         <v>1.3332999999999999</v>
       </c>
-      <c r="F24" s="1">
-        <v>2007</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H24" s="1">
-        <v>648008</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2014</v>
       </c>
@@ -2282,20 +2159,14 @@
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="1">
         <v>105.33329999999999</v>
       </c>
-      <c r="F25" s="1">
-        <v>2008</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H25" s="1">
-        <v>630438</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2014</v>
       </c>
@@ -2305,20 +2176,14 @@
       <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="1">
         <v>56</v>
       </c>
-      <c r="F26" s="1">
-        <v>2009</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H26" s="1">
-        <v>439678</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2014</v>
       </c>
@@ -2328,20 +2193,14 @@
       <c r="C27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="1">
         <v>28</v>
       </c>
-      <c r="F27" s="1">
-        <v>2010</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H27" s="1">
-        <v>538291</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2014</v>
       </c>
@@ -2351,20 +2210,14 @@
       <c r="C28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="1">
         <v>21.333300000000001</v>
       </c>
-      <c r="F28" s="1">
-        <v>2011</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H28" s="1">
-        <v>364416</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2014</v>
       </c>
@@ -2374,20 +2227,14 @@
       <c r="C29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="1">
         <v>1.3332999999999999</v>
       </c>
-      <c r="F29" s="1">
-        <v>2012</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H29" s="1">
-        <v>411036</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2014</v>
       </c>
@@ -2397,20 +2244,14 @@
       <c r="C30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="1">
         <v>0</v>
       </c>
-      <c r="F30" s="1">
-        <v>2013</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H30" s="1">
-        <v>624801</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2014</v>
       </c>
@@ -2420,20 +2261,14 @@
       <c r="C31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="1">
-        <v>12</v>
-      </c>
-      <c r="F31" s="1">
-        <v>2014</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H31" s="1">
-        <v>328527</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2014</v>
       </c>
@@ -2443,20 +2278,14 @@
       <c r="C32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="1">
         <v>173.33330000000001</v>
       </c>
-      <c r="F32" s="1">
-        <v>1998</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H32" s="1">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2014</v>
       </c>
@@ -2466,20 +2295,14 @@
       <c r="C33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="1">
         <v>176</v>
       </c>
-      <c r="F33" s="1">
-        <v>1999</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H33" s="1">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2014</v>
       </c>
@@ -2489,20 +2312,14 @@
       <c r="C34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="1">
         <v>4</v>
       </c>
-      <c r="F34" s="1">
-        <v>2000</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H34" s="1">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2014</v>
       </c>
@@ -2512,20 +2329,14 @@
       <c r="C35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="1">
         <v>6.6666999999999996</v>
       </c>
-      <c r="F35" s="1">
-        <v>2001</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H35" s="1">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2014</v>
       </c>
@@ -2535,20 +2346,14 @@
       <c r="C36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="1">
         <v>6.6666999999999996</v>
       </c>
-      <c r="F36" s="1">
-        <v>2002</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H36" s="1">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2014</v>
       </c>
@@ -2558,20 +2363,14 @@
       <c r="C37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="1">
         <v>37.333300000000001</v>
       </c>
-      <c r="F37" s="1">
-        <v>2003</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H37" s="1">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2014</v>
       </c>
@@ -2581,20 +2380,14 @@
       <c r="C38" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" s="1">
         <v>33.333300000000001</v>
       </c>
-      <c r="F38" s="1">
-        <v>2004</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H38" s="1">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2014</v>
       </c>
@@ -2604,20 +2397,14 @@
       <c r="C39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" s="1">
         <v>0</v>
       </c>
-      <c r="F39" s="1">
-        <v>2005</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H39" s="1">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2014</v>
       </c>
@@ -2627,20 +2414,14 @@
       <c r="C40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" s="1">
         <v>0</v>
       </c>
-      <c r="F40" s="1">
-        <v>2006</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H40" s="1">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2014</v>
       </c>
@@ -2650,20 +2431,14 @@
       <c r="C41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="1">
         <v>0</v>
       </c>
-      <c r="F41" s="1">
-        <v>2007</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H41" s="1">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2014</v>
       </c>
@@ -2673,20 +2448,14 @@
       <c r="C42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="1">
         <v>37.333300000000001</v>
       </c>
-      <c r="F42" s="1">
-        <v>2008</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H42" s="1">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2014</v>
       </c>
@@ -2696,764 +2465,1880 @@
       <c r="C43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="1">
         <v>2.6667000000000001</v>
       </c>
-      <c r="F43" s="1">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="1">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" s="1">
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" s="1">
+        <v>5.46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" s="1">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E52" s="2">
+        <v>928879</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E53" s="2">
+        <v>1024712</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E54" s="2">
+        <v>930173</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E55" s="2">
+        <v>876711</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E56" s="2">
+        <v>924396</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
         <v>2009</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="B57" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E57" s="2">
+        <v>642860</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E58" s="2">
+        <v>873044</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E59" s="2">
+        <v>666209</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E60" s="2">
+        <v>693020</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E61" s="2">
+        <v>919883</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E62" s="2">
+        <v>636412</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E63" s="1">
+        <v>654970</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E64" s="1">
+        <v>741061</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E65" s="1">
+        <v>689075</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E66" s="1">
+        <v>648008</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E67" s="1">
+        <v>630438</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E68" s="1">
+        <v>439678</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E69" s="1">
+        <v>538291</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E70" s="1">
+        <v>364416</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E71" s="1">
+        <v>411036</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E72" s="1">
+        <v>624801</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E73" s="1">
+        <v>328527</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>1998</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H43" s="1">
+      <c r="E74" s="1">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E75" s="1">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E76" s="1">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E77" s="1">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E78" s="1">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E79" s="1">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E80" s="1">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E81" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E82" s="1">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E83" s="1">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E84" s="1">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E85" s="1">
         <v>610</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F44" s="1">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
         <v>2010</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="B86" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H44" s="1">
+      <c r="E86" s="1">
         <v>503</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F45" s="1">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
         <v>2011</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="B87" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H45" s="1">
+      <c r="E87" s="1">
         <v>441</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F46" s="1">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
         <v>2012</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="B88" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H46" s="1">
+      <c r="E88" s="1">
         <v>573</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F47" s="1">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
         <v>2013</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="B89" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H47" s="1">
+      <c r="E89" s="1">
         <v>519</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F48" s="1">
-        <v>2014</v>
-      </c>
-      <c r="G48" s="1" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H48" s="1">
+      <c r="E90" s="1">
         <v>504</v>
       </c>
     </row>
-    <row r="49" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F49" s="1">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
         <v>2015</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="B91" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H49" s="1">
+      <c r="E91" s="1">
         <v>742</v>
       </c>
     </row>
-    <row r="50" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F50" s="1">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
         <v>1998</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="B92" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H50" s="1">
+      <c r="E92" s="1">
         <v>618</v>
       </c>
     </row>
-    <row r="51" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F51" s="1">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
         <v>1999</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="B93" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H51" s="1">
+      <c r="E93" s="1">
         <v>563</v>
       </c>
     </row>
-    <row r="52" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F52" s="1">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
         <v>2000</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="B94" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H52" s="1">
+      <c r="E94" s="1">
         <v>632</v>
       </c>
     </row>
-    <row r="53" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F53" s="1">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
         <v>2001</v>
       </c>
-      <c r="G53" s="1" t="s">
+      <c r="B95" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H53" s="1">
+      <c r="E95" s="1">
         <v>446</v>
       </c>
     </row>
-    <row r="54" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F54" s="1">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
         <v>2002</v>
       </c>
-      <c r="G54" s="1" t="s">
+      <c r="B96" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H54" s="1">
+      <c r="E96" s="1">
         <v>622</v>
       </c>
     </row>
-    <row r="55" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F55" s="1">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
         <v>2003</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="B97" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H55" s="1">
+      <c r="E97" s="1">
         <v>460</v>
       </c>
     </row>
-    <row r="56" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F56" s="1">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
         <v>2004</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="B98" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H56" s="1">
+      <c r="E98" s="1">
         <v>464</v>
       </c>
     </row>
-    <row r="57" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F57" s="1">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
         <v>2005</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="B99" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H57" s="1">
+      <c r="E99" s="1">
         <v>352</v>
       </c>
     </row>
-    <row r="58" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F58" s="1">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
         <v>2006</v>
       </c>
-      <c r="G58" s="1" t="s">
+      <c r="B100" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D100" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H58" s="1">
+      <c r="E100" s="1">
         <v>289</v>
       </c>
     </row>
-    <row r="59" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F59" s="1">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
         <v>2007</v>
       </c>
-      <c r="G59" s="1" t="s">
+      <c r="B101" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H59" s="1">
+      <c r="E101" s="1">
         <v>494</v>
       </c>
     </row>
-    <row r="60" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F60" s="1">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
         <v>2008</v>
       </c>
-      <c r="G60" s="1" t="s">
+      <c r="B102" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H60" s="1">
+      <c r="E102" s="1">
         <v>290</v>
       </c>
     </row>
-    <row r="61" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F61" s="1">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
         <v>2009</v>
       </c>
-      <c r="G61" s="1" t="s">
+      <c r="B103" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H61" s="1">
+      <c r="E103" s="1">
         <v>335</v>
       </c>
     </row>
-    <row r="62" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F62" s="1">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
         <v>2010</v>
       </c>
-      <c r="G62" s="1" t="s">
+      <c r="B104" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H62" s="1">
+      <c r="E104" s="1">
         <v>304</v>
       </c>
     </row>
-    <row r="63" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F63" s="1">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
         <v>2011</v>
       </c>
-      <c r="G63" s="1" t="s">
+      <c r="B105" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H63" s="1">
+      <c r="E105" s="1">
         <v>262</v>
       </c>
     </row>
-    <row r="64" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F64" s="1">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
         <v>2012</v>
       </c>
-      <c r="G64" s="1" t="s">
+      <c r="B106" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H64" s="1">
+      <c r="E106" s="1">
         <v>358</v>
       </c>
     </row>
-    <row r="65" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F65" s="1">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
         <v>2013</v>
       </c>
-      <c r="G65" s="1" t="s">
+      <c r="B107" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D107" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H65" s="1">
+      <c r="E107" s="1">
         <v>349</v>
       </c>
     </row>
-    <row r="66" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F66" s="1">
-        <v>2014</v>
-      </c>
-      <c r="G66" s="1" t="s">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H66" s="1">
+      <c r="E108" s="1">
         <v>320</v>
       </c>
     </row>
-    <row r="67" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F67" s="1">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
         <v>2015</v>
       </c>
-      <c r="G67" s="1" t="s">
+      <c r="B109" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H67" s="1">
+      <c r="E109" s="1">
         <v>513</v>
       </c>
     </row>
-    <row r="68" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F68" s="1">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
         <v>1998</v>
       </c>
-      <c r="G68" s="1" t="s">
+      <c r="B110" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D110" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H68" s="1">
+      <c r="E110" s="1">
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F69" s="1">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
         <v>1999</v>
       </c>
-      <c r="G69" s="1" t="s">
+      <c r="B111" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H69" s="1">
+      <c r="E111" s="1">
         <v>63</v>
       </c>
     </row>
-    <row r="70" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F70" s="1">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
         <v>2000</v>
       </c>
-      <c r="G70" s="1" t="s">
+      <c r="B112" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H70" s="1">
+      <c r="E112" s="1">
         <v>58</v>
       </c>
     </row>
-    <row r="71" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F71" s="1">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
         <v>2001</v>
       </c>
-      <c r="G71" s="1" t="s">
+      <c r="B113" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H71" s="1">
+      <c r="E113" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="72" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F72" s="1">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
         <v>2002</v>
       </c>
-      <c r="G72" s="1" t="s">
+      <c r="B114" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H72" s="1">
+      <c r="E114" s="1">
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F73" s="1">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
         <v>2003</v>
       </c>
-      <c r="G73" s="1" t="s">
+      <c r="B115" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H73" s="1">
+      <c r="E115" s="1">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F74" s="1">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
         <v>2004</v>
       </c>
-      <c r="G74" s="1" t="s">
+      <c r="B116" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H74" s="1">
+      <c r="E116" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="75" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F75" s="1">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
         <v>2005</v>
       </c>
-      <c r="G75" s="1" t="s">
+      <c r="B117" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H75" s="1">
+      <c r="E117" s="1">
         <v>98</v>
       </c>
     </row>
-    <row r="76" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F76" s="1">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
         <v>2006</v>
       </c>
-      <c r="G76" s="1" t="s">
+      <c r="B118" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H76" s="1">
+      <c r="E118" s="1">
         <v>108</v>
       </c>
     </row>
-    <row r="77" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F77" s="1">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
         <v>2007</v>
       </c>
-      <c r="G77" s="1" t="s">
+      <c r="B119" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H77" s="1">
+      <c r="E119" s="1">
         <v>108</v>
       </c>
     </row>
-    <row r="78" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F78" s="1">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
         <v>2008</v>
       </c>
-      <c r="G78" s="1" t="s">
+      <c r="B120" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H78" s="1">
+      <c r="E120" s="1">
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F79" s="1">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
         <v>2010</v>
       </c>
-      <c r="G79" s="1" t="s">
+      <c r="B121" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D121" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H79" s="1">
+      <c r="E121" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="80" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F80" s="1">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
         <v>2011</v>
       </c>
-      <c r="G80" s="1" t="s">
+      <c r="B122" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D122" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H80" s="1">
+      <c r="E122" s="1">
         <v>108</v>
       </c>
     </row>
-    <row r="81" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F81" s="1">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
         <v>2012</v>
       </c>
-      <c r="G81" s="1" t="s">
+      <c r="B123" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H81" s="1">
+      <c r="E123" s="1">
         <v>126</v>
       </c>
     </row>
-    <row r="82" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F82" s="1">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
         <v>2013</v>
       </c>
-      <c r="G82" s="1" t="s">
+      <c r="B124" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H82" s="1">
+      <c r="E124" s="1">
         <v>138</v>
       </c>
     </row>
-    <row r="83" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F83" s="1">
-        <v>2014</v>
-      </c>
-      <c r="G83" s="1" t="s">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D125" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H83" s="1">
+      <c r="E125" s="1">
         <v>127</v>
       </c>
     </row>
-    <row r="84" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F84" s="1">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
         <v>1998</v>
       </c>
-      <c r="G84" s="1" t="s">
+      <c r="B126" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H84" s="1">
+      <c r="E126" s="1">
         <v>0.56269999999999998</v>
       </c>
     </row>
-    <row r="85" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F85" s="1">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
         <v>1999</v>
       </c>
-      <c r="G85" s="1" t="s">
+      <c r="B127" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D127" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H85" s="1">
+      <c r="E127" s="1">
         <v>0.52210000000000001</v>
       </c>
     </row>
-    <row r="86" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F86" s="1">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
         <v>2000</v>
       </c>
-      <c r="G86" s="1" t="s">
+      <c r="B128" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D128" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H86" s="1">
+      <c r="E128" s="1">
         <v>0.49419999999999997</v>
       </c>
     </row>
-    <row r="87" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F87" s="1">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
         <v>2001</v>
       </c>
-      <c r="G87" s="1" t="s">
+      <c r="B129" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D129" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H87" s="1">
+      <c r="E129" s="1">
         <v>0.49830000000000002</v>
       </c>
     </row>
-    <row r="88" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F88" s="1">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
         <v>2002</v>
       </c>
-      <c r="G88" s="1" t="s">
+      <c r="B130" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D130" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H88" s="1">
+      <c r="E130" s="1">
         <v>0.47949999999999998</v>
       </c>
     </row>
-    <row r="89" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F89" s="1">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
         <v>2003</v>
       </c>
-      <c r="G89" s="1" t="s">
+      <c r="B131" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D131" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H89" s="1">
+      <c r="E131" s="1">
         <v>0.48020000000000002</v>
       </c>
     </row>
-    <row r="90" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F90" s="1">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
         <v>2004</v>
       </c>
-      <c r="G90" s="1" t="s">
+      <c r="B132" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D132" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H90" s="1">
+      <c r="E132" s="1">
         <v>0.47470000000000001</v>
       </c>
     </row>
-    <row r="91" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F91" s="1">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
         <v>2005</v>
       </c>
-      <c r="G91" s="1" t="s">
+      <c r="B133" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D133" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H91" s="1">
+      <c r="E133" s="1">
         <v>0.52949999999999997</v>
       </c>
     </row>
-    <row r="92" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F92" s="1">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
         <v>2006</v>
       </c>
-      <c r="G92" s="1" t="s">
+      <c r="B134" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D134" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H92" s="1">
+      <c r="E134" s="1">
         <v>0.51419999999999999</v>
       </c>
     </row>
-    <row r="93" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F93" s="1">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
         <v>2007</v>
       </c>
-      <c r="G93" s="1" t="s">
+      <c r="B135" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D135" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H93" s="1">
+      <c r="E135" s="1">
         <v>0.46760000000000002</v>
       </c>
     </row>
-    <row r="94" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F94" s="1">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
         <v>2008</v>
       </c>
-      <c r="G94" s="1" t="s">
+      <c r="B136" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D136" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H94" s="1">
+      <c r="E136" s="1">
         <v>0.497</v>
       </c>
     </row>
-    <row r="95" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F95" s="1">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
         <v>2009</v>
       </c>
-      <c r="G95" s="1" t="s">
+      <c r="B137" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D137" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H95" s="1">
+      <c r="E137" s="1">
         <v>0.53580000000000005</v>
       </c>
     </row>
-    <row r="96" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F96" s="1">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
         <v>2010</v>
       </c>
-      <c r="G96" s="1" t="s">
+      <c r="B138" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D138" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H96" s="1">
+      <c r="E138" s="1">
         <v>0.60050000000000003</v>
       </c>
     </row>
-    <row r="97" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F97" s="1">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
         <v>2011</v>
       </c>
-      <c r="G97" s="1" t="s">
+      <c r="B139" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D139" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H97" s="1">
+      <c r="E139" s="1">
         <v>0.58360000000000001</v>
       </c>
     </row>
-    <row r="98" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F98" s="1">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
         <v>2012</v>
       </c>
-      <c r="G98" s="1" t="s">
+      <c r="B140" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D140" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H98" s="1">
+      <c r="E140" s="1">
         <v>0.57930000000000004</v>
       </c>
     </row>
-    <row r="99" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F99" s="1">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
         <v>2013</v>
       </c>
-      <c r="G99" s="1" t="s">
+      <c r="B141" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D141" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H99" s="1">
+      <c r="E141" s="1">
         <v>0.55830000000000002</v>
       </c>
     </row>
-    <row r="100" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F100" s="1">
-        <v>2014</v>
-      </c>
-      <c r="G100" s="1" t="s">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D142" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H100" s="1">
+      <c r="E142" s="1">
         <v>0.56640000000000001</v>
       </c>
     </row>
-    <row r="101" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F101" s="1">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
         <v>2004</v>
       </c>
-      <c r="G101" s="1" t="s">
+      <c r="B143" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D143" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H101" s="1">
+      <c r="E143" s="1">
         <v>19.739999999999998</v>
       </c>
     </row>
-    <row r="102" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F102" s="1">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
         <v>2005</v>
       </c>
-      <c r="G102" s="1" t="s">
+      <c r="B144" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D144" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H102" s="1">
+      <c r="E144" s="1">
         <v>19.22</v>
       </c>
     </row>
-    <row r="103" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F103" s="1">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
         <v>2006</v>
       </c>
-      <c r="G103" s="1" t="s">
+      <c r="B145" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D145" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H103" s="1">
+      <c r="E145" s="1">
         <v>18.690000000000001</v>
       </c>
     </row>
-    <row r="104" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F104" s="1">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
         <v>2007</v>
       </c>
-      <c r="G104" s="1" t="s">
+      <c r="B146" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D146" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H104" s="1">
+      <c r="E146" s="1">
         <v>21.25</v>
       </c>
     </row>
-    <row r="105" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F105" s="1">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
         <v>2008</v>
       </c>
-      <c r="G105" s="1" t="s">
+      <c r="B147" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D147" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H105" s="1">
+      <c r="E147" s="1">
         <v>19.63</v>
       </c>
     </row>
-    <row r="106" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F106" s="1">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
         <v>2009</v>
       </c>
-      <c r="G106" s="1" t="s">
+      <c r="B148" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D148" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H106" s="1">
+      <c r="E148" s="1">
         <v>19.12</v>
       </c>
     </row>
-    <row r="107" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F107" s="1">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
         <v>2010</v>
       </c>
-      <c r="G107" s="1" t="s">
+      <c r="B149" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D149" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H107" s="1">
+      <c r="E149" s="1">
         <v>18.95</v>
       </c>
     </row>
-    <row r="108" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F108" s="1">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
         <v>2011</v>
       </c>
-      <c r="G108" s="1" t="s">
+      <c r="B150" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D150" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H108" s="1">
+      <c r="E150" s="1">
         <v>19.079999999999998</v>
       </c>
     </row>
-    <row r="109" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F109" s="1">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
         <v>2012</v>
       </c>
-      <c r="G109" s="1" t="s">
+      <c r="B151" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D151" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H109" s="1">
+      <c r="E151" s="1">
         <v>19.93</v>
       </c>
     </row>
-    <row r="110" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F110" s="1">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
         <v>2013</v>
       </c>
-      <c r="G110" s="1" t="s">
+      <c r="B152" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D152" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H110" s="1">
+      <c r="E152" s="1">
         <v>19.57</v>
       </c>
     </row>
-    <row r="111" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F111" s="1">
-        <v>2014</v>
-      </c>
-      <c r="G111" s="1" t="s">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D153" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H111" s="1">
+      <c r="E153" s="1">
         <v>19.45</v>
       </c>
     </row>

</xml_diff>